<commit_message>
cleaned up nan cells, and updated tabula EOD report
</commit_message>
<xml_diff>
--- a/tabula-END OF DAY REPORT - XYZ COMPANY.xlsx
+++ b/tabula-END OF DAY REPORT - XYZ COMPANY.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfon\Documents\Automation_Project\First-automation-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F2EE6DB-8FAD-4702-98B0-24401F4B9260}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6AEEFE7-DFEE-4C71-810D-0DFD4B28A784}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10635" yWindow="825" windowWidth="15375" windowHeight="7875"/>
+    <workbookView xWindow="4125" yWindow="1365" windowWidth="15375" windowHeight="7875" xr2:uid="{9EDECE3A-99CC-4EFF-BF28-3653B8559CCF}"/>
   </bookViews>
   <sheets>
-    <sheet name="tabula-END OF DAY REPORT - XYZ " sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -214,9 +225,6 @@
     <t>03/16/2020 0001492292</t>
   </si>
   <si>
-    <t>G1651A</t>
-  </si>
-  <si>
     <t>END OF DAY REPORT</t>
   </si>
   <si>
@@ -248,16 +256,19 @@
   </si>
   <si>
     <t>GRAND TOTAL: $468,180.78</t>
+  </si>
+  <si>
+    <t>$250.00 G1651A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,316 +276,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -582,206 +293,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1092,10 +614,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE4B6C9-08E4-4810-863E-65FA8B0BABA9}">
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1143,6 +667,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>81730</v>
+      </c>
       <c r="B6">
         <v>126104</v>
       </c>
@@ -1157,6 +684,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>81730</v>
+      </c>
       <c r="B7">
         <v>139729</v>
       </c>
@@ -1171,6 +701,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>81730</v>
+      </c>
       <c r="B8">
         <v>415802</v>
       </c>
@@ -1185,6 +718,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>81730</v>
+      </c>
       <c r="B9">
         <v>1018908</v>
       </c>
@@ -1199,6 +735,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>81730</v>
+      </c>
       <c r="B10">
         <v>1065569</v>
       </c>
@@ -1217,17 +756,10 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>81730</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>81733</v>
-      </c>
-    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>81733</v>
+      </c>
       <c r="B14">
         <v>129188</v>
       </c>
@@ -1242,6 +774,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>81733</v>
+      </c>
       <c r="B15">
         <v>141077</v>
       </c>
@@ -1256,6 +791,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>81733</v>
+      </c>
       <c r="B16">
         <v>149443</v>
       </c>
@@ -1269,7 +807,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>81733</v>
+      </c>
       <c r="B17">
         <v>163549</v>
       </c>
@@ -1283,7 +824,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>81733</v>
+      </c>
       <c r="B18">
         <v>302068</v>
       </c>
@@ -1297,7 +841,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>81733</v>
+      </c>
       <c r="B19">
         <v>318123</v>
       </c>
@@ -1311,7 +858,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>81733</v>
+      </c>
       <c r="B20">
         <v>413376</v>
       </c>
@@ -1325,7 +875,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>81733</v>
+      </c>
       <c r="B21">
         <v>413376</v>
       </c>
@@ -1339,7 +892,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>81733</v>
+      </c>
       <c r="B22">
         <v>424431</v>
       </c>
@@ -1353,7 +909,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>81733</v>
+      </c>
       <c r="B23">
         <v>432540</v>
       </c>
@@ -1367,7 +926,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>81733</v>
+      </c>
       <c r="B24">
         <v>432540</v>
       </c>
@@ -1381,7 +943,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>81733</v>
+      </c>
       <c r="B25">
         <v>810469</v>
       </c>
@@ -1395,7 +960,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>81733</v>
+      </c>
       <c r="B26">
         <v>824824</v>
       </c>
@@ -1409,7 +977,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>81733</v>
+      </c>
       <c r="B27">
         <v>834696</v>
       </c>
@@ -1423,7 +994,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>81733</v>
+      </c>
       <c r="B28">
         <v>837873</v>
       </c>
@@ -1437,7 +1011,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>81733</v>
+      </c>
       <c r="B29">
         <v>867566</v>
       </c>
@@ -1451,7 +1028,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>81733</v>
+      </c>
       <c r="B30">
         <v>873349</v>
       </c>
@@ -1465,7 +1045,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>81733</v>
+      </c>
       <c r="B31">
         <v>877756</v>
       </c>
@@ -1479,7 +1062,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>81733</v>
+      </c>
       <c r="B32">
         <v>907172</v>
       </c>
@@ -1493,7 +1079,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>81733</v>
+      </c>
       <c r="B33">
         <v>907172</v>
       </c>
@@ -1507,7 +1096,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>81733</v>
+      </c>
       <c r="B34">
         <v>914864</v>
       </c>
@@ -1521,7 +1113,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>81733</v>
+      </c>
       <c r="B35">
         <v>916980</v>
       </c>
@@ -1535,7 +1130,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>81733</v>
+      </c>
       <c r="B36">
         <v>936797</v>
       </c>
@@ -1549,7 +1147,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>81733</v>
+      </c>
       <c r="B37">
         <v>976785</v>
       </c>
@@ -1563,7 +1164,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>81733</v>
+      </c>
       <c r="B38">
         <v>976785</v>
       </c>
@@ -1577,7 +1181,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>81733</v>
+      </c>
       <c r="B39">
         <v>993472</v>
       </c>
@@ -1591,7 +1198,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>81733</v>
+      </c>
       <c r="B40">
         <v>1001448</v>
       </c>
@@ -1605,7 +1215,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>81733</v>
+      </c>
       <c r="B41">
         <v>1002032</v>
       </c>
@@ -1619,7 +1232,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>81733</v>
+      </c>
       <c r="B42">
         <v>1025858</v>
       </c>
@@ -1633,7 +1249,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>81733</v>
+      </c>
       <c r="B43">
         <v>1035053</v>
       </c>
@@ -1647,7 +1266,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>81733</v>
+      </c>
       <c r="B44">
         <v>1035701</v>
       </c>
@@ -1661,7 +1283,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>81733</v>
+      </c>
       <c r="B45">
         <v>1035704</v>
       </c>
@@ -1675,7 +1300,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>81733</v>
+      </c>
       <c r="B46">
         <v>1039113</v>
       </c>
@@ -1689,7 +1317,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>81733</v>
+      </c>
       <c r="B47">
         <v>1043815</v>
       </c>
@@ -1703,7 +1334,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>81733</v>
+      </c>
       <c r="B48">
         <v>1054901</v>
       </c>
@@ -1717,46 +1351,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <v>466025.78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>81736</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>134593</v>
-      </c>
-      <c r="C51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="2">
-        <v>250</v>
-      </c>
-      <c r="E51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>43910</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1767,61 +1382,87 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>81736</v>
+      </c>
       <c r="B56">
         <v>164304</v>
       </c>
       <c r="C56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
         <v>67</v>
       </c>
-      <c r="D56" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>81736</v>
+      </c>
       <c r="B57">
         <v>164304</v>
       </c>
       <c r="C57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" t="s">
         <v>69</v>
       </c>
-      <c r="D57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>81736</v>
+      </c>
       <c r="B58">
         <v>820366</v>
       </c>
       <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" t="s">
         <v>71</v>
       </c>
-      <c r="D58" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>81736</v>
+      </c>
       <c r="B59">
         <v>828968</v>
       </c>
       <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
         <v>73</v>
       </c>
-      <c r="D59" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>81736</v>
+      </c>
+      <c r="B60">
+        <v>134593</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D60" s="2">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>